<commit_message>
added sector sheets, TXN, yield curve updated 3/15/24
</commit_message>
<xml_diff>
--- a/00Dashboard.xlsx
+++ b/00Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlshe\Documents\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECC4D9B-0284-43DE-9107-B8AB741A8F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8185CBB3-E1C1-4824-A973-E06AAD778BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4588CD03-294E-421F-A4EF-704A3E6AC4BE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4588CD03-294E-421F-A4EF-704A3E6AC4BE}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Bond Yields" sheetId="2" r:id="rId1"/>
@@ -5593,7 +5593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78598AC-1488-4768-97DC-A6CDF693DFF7}">
   <dimension ref="B3:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -6564,11 +6564,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C57CBD6-140C-4F1E-BA61-90A42EC2B8A9}">
   <dimension ref="A2:W30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8252,7 +8252,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" t="e" vm="21">
+      <c r="B23" s="21" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
       <c r="C23" s="26">
@@ -8377,10 +8377,11 @@
     <hyperlink ref="B20" r:id="rId18" display="COTY.xlsx" xr:uid="{BCF85E8D-3A96-41F7-96A9-57C75D61AF99}"/>
     <hyperlink ref="B22" r:id="rId19" display="GOOGL.xlsx" xr:uid="{B14E25EB-BD9A-46E4-A64C-5D732F749CCC}"/>
     <hyperlink ref="B21" r:id="rId20" display="TM.xlsx" xr:uid="{A9C43251-15F2-4E54-83A1-C629C893BBD0}"/>
+    <hyperlink ref="B23" r:id="rId21" display="TXN.xlsx" xr:uid="{C9BF9B6C-43E9-4E95-BC3E-4165AEC1FF9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
-  <legacyDrawing r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
+  <legacyDrawing r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>